<commit_message>
##olease enter the commit message for your changes. Lines starting
</commit_message>
<xml_diff>
--- a/DataTables/catalog_final.xlsx
+++ b/DataTables/catalog_final.xlsx
@@ -1,14 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MY091D\Downloads\dApp\deployment\DataTables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\create-react-app\my-app\DataTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{81A067AF-DAFA-4699-9E0B-85D0CA7788E4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160"/>
   </bookViews>
@@ -43,9 +42,6 @@
     <t>titlekeyword</t>
   </si>
   <si>
-    <t>category</t>
-  </si>
-  <si>
     <t>comments</t>
   </si>
   <si>
@@ -1960,12 +1956,15 @@
   </si>
   <si>
     <t>Born to survivalists in the mountains of Idaho, Tara Westover was seventeen the first time she set foot in a classroom. Her family was so isolated from mainstream society that there was no one to ensure the children received an education, and no one to intervene when one of Tara’s older brothers became violent. When another brother got himself into college, Tara decided to try a new kind of life. Her quest for knowledge transformed her, taking her over oceans and across continents, to Harvard and to Cambridge University. Only then would she wonder if she’d traveled too far, if there was still a way home.</t>
+  </si>
+  <si>
+    <t>genre</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2806,7 +2805,7 @@
   <dimension ref="A1:J120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2818,7 +2817,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -2842,10 +2841,10 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
+        <v>645</v>
+      </c>
+      <c r="J1" t="s">
         <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2853,31 +2852,31 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>15</v>
-      </c>
-      <c r="J2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2885,28 +2884,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="G3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>603</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>20</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>21</v>
-      </c>
-      <c r="I3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2914,28 +2913,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="G4" t="s">
         <v>24</v>
       </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>604</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>25</v>
       </c>
-      <c r="H4" t="s">
-        <v>26</v>
-      </c>
       <c r="I4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2943,28 +2942,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" t="s">
         <v>28</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>29</v>
       </c>
-      <c r="H5" t="s">
-        <v>30</v>
-      </c>
       <c r="I5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -2972,28 +2971,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
         <v>31</v>
-      </c>
-      <c r="C6" t="s">
-        <v>32</v>
       </c>
       <c r="D6">
         <v>2002</v>
       </c>
       <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" t="s">
         <v>34</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>35</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>36</v>
-      </c>
-      <c r="I6" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3001,28 +3000,28 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
         <v>38</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
         <v>39</v>
       </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="F7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" t="s">
         <v>41</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>42</v>
       </c>
-      <c r="H7" t="s">
-        <v>43</v>
-      </c>
       <c r="I7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3030,28 +3029,28 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
         <v>44</v>
       </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>45</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>46</v>
-      </c>
-      <c r="I8" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3059,28 +3058,28 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" t="s">
         <v>48</v>
-      </c>
-      <c r="C9" t="s">
-        <v>49</v>
       </c>
       <c r="D9">
         <v>2001</v>
       </c>
       <c r="E9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>51</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>52</v>
-      </c>
-      <c r="I9" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="180" x14ac:dyDescent="0.25">
@@ -3088,28 +3087,28 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" t="s">
         <v>54</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
         <v>55</v>
       </c>
-      <c r="D10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="F10" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" t="s">
         <v>57</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>58</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>59</v>
-      </c>
-      <c r="I10" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3117,28 +3116,28 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" t="s">
         <v>61</v>
-      </c>
-      <c r="C11" t="s">
-        <v>62</v>
       </c>
       <c r="D11">
         <v>2003</v>
       </c>
       <c r="E11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" t="s">
         <v>64</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>65</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>66</v>
-      </c>
-      <c r="I11" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3146,28 +3145,28 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" t="s">
         <v>68</v>
-      </c>
-      <c r="C12" t="s">
-        <v>69</v>
       </c>
       <c r="D12">
         <v>2003</v>
       </c>
       <c r="E12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="G12" t="s">
         <v>70</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>605</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>71</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>72</v>
-      </c>
-      <c r="I12" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3175,28 +3174,28 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" t="s">
         <v>74</v>
-      </c>
-      <c r="C13" t="s">
-        <v>75</v>
       </c>
       <c r="D13">
         <v>2007</v>
       </c>
       <c r="E13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" t="s">
         <v>77</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>78</v>
       </c>
-      <c r="H13" t="s">
-        <v>79</v>
-      </c>
       <c r="I13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3204,28 +3203,28 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" t="s">
         <v>81</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>82</v>
       </c>
-      <c r="H14" t="s">
-        <v>83</v>
-      </c>
       <c r="I14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3233,28 +3232,28 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C15" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" t="s">
         <v>85</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>86</v>
       </c>
-      <c r="H15" t="s">
-        <v>87</v>
-      </c>
       <c r="I15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="180" x14ac:dyDescent="0.25">
@@ -3262,28 +3261,28 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="G16" t="s">
         <v>88</v>
       </c>
-      <c r="C16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>606</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>89</v>
       </c>
-      <c r="H16" t="s">
-        <v>90</v>
-      </c>
       <c r="I16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -3291,28 +3290,28 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C17" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" t="s">
-        <v>40</v>
-      </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" t="s">
         <v>92</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>93</v>
       </c>
-      <c r="H17" t="s">
-        <v>94</v>
-      </c>
       <c r="I17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -3320,28 +3319,28 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C18" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" t="s">
-        <v>40</v>
-      </c>
-      <c r="F18" s="1" t="s">
+      <c r="G18" t="s">
         <v>96</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>97</v>
       </c>
-      <c r="H18" t="s">
-        <v>98</v>
-      </c>
       <c r="I18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="195" x14ac:dyDescent="0.25">
@@ -3349,28 +3348,28 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" t="s">
         <v>99</v>
-      </c>
-      <c r="C19" t="s">
-        <v>100</v>
       </c>
       <c r="D19">
         <v>1975</v>
       </c>
       <c r="E19" t="s">
+        <v>100</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="G19" t="s">
         <v>101</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>641</v>
-      </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>102</v>
       </c>
-      <c r="H19" t="s">
-        <v>103</v>
-      </c>
       <c r="I19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="150" x14ac:dyDescent="0.25">
@@ -3378,28 +3377,28 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" t="s">
         <v>104</v>
-      </c>
-      <c r="C20" t="s">
-        <v>105</v>
       </c>
       <c r="D20">
         <v>2002</v>
       </c>
       <c r="E20" t="s">
+        <v>105</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="G20" t="s">
         <v>107</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>108</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>109</v>
-      </c>
-      <c r="I20" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -3407,28 +3406,28 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C21" t="s">
         <v>111</v>
-      </c>
-      <c r="C21" t="s">
-        <v>112</v>
       </c>
       <c r="D21">
         <v>1998</v>
       </c>
       <c r="E21" t="s">
+        <v>112</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="G21" t="s">
         <v>114</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>115</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>116</v>
-      </c>
-      <c r="I21" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -3436,28 +3435,28 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" t="s">
         <v>118</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" t="s">
-        <v>56</v>
-      </c>
-      <c r="F22" s="1" t="s">
+      <c r="G22" t="s">
         <v>120</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>121</v>
       </c>
-      <c r="H22" t="s">
-        <v>122</v>
-      </c>
       <c r="I22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -3465,28 +3464,28 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C23" t="s">
         <v>123</v>
-      </c>
-      <c r="C23" t="s">
-        <v>124</v>
       </c>
       <c r="D23">
         <v>1995</v>
       </c>
       <c r="E23" t="s">
+        <v>124</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="G23" t="s">
         <v>125</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>607</v>
-      </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>126</v>
       </c>
-      <c r="H23" t="s">
-        <v>127</v>
-      </c>
       <c r="I23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3494,28 +3493,28 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C24" t="s">
         <v>128</v>
-      </c>
-      <c r="C24" t="s">
-        <v>129</v>
       </c>
       <c r="D24">
         <v>2006</v>
       </c>
       <c r="E24" t="s">
+        <v>129</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="G24" t="s">
         <v>131</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>132</v>
       </c>
-      <c r="H24" t="s">
-        <v>133</v>
-      </c>
       <c r="I24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3523,28 +3522,28 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C25" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F25" s="1" t="s">
+      <c r="G25" t="s">
         <v>135</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>136</v>
       </c>
-      <c r="H25" t="s">
-        <v>137</v>
-      </c>
       <c r="I25" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3552,28 +3551,28 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C26" t="s">
         <v>138</v>
-      </c>
-      <c r="C26" t="s">
-        <v>139</v>
       </c>
       <c r="D26">
         <v>2012</v>
       </c>
       <c r="E26" t="s">
+        <v>139</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" t="s">
         <v>140</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>141</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>142</v>
-      </c>
-      <c r="I26" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="195" x14ac:dyDescent="0.25">
@@ -3581,28 +3580,28 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C27" t="s">
         <v>144</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" t="s">
+        <v>55</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="G27" t="s">
         <v>145</v>
       </c>
-      <c r="D27" t="s">
-        <v>11</v>
-      </c>
-      <c r="E27" t="s">
-        <v>56</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>608</v>
-      </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>146</v>
       </c>
-      <c r="H27" t="s">
-        <v>147</v>
-      </c>
       <c r="I27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3610,28 +3609,28 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C28" t="s">
-        <v>11</v>
-      </c>
-      <c r="D28" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" t="s">
-        <v>11</v>
-      </c>
-      <c r="F28" s="1" t="s">
+      <c r="G28" t="s">
         <v>149</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>150</v>
       </c>
-      <c r="H28" t="s">
-        <v>151</v>
-      </c>
       <c r="I28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="210" x14ac:dyDescent="0.25">
@@ -3639,28 +3638,28 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C29" t="s">
         <v>152</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" t="s">
+        <v>55</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="G29" t="s">
         <v>153</v>
       </c>
-      <c r="D29" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29" t="s">
-        <v>56</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>609</v>
-      </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>154</v>
       </c>
-      <c r="H29" t="s">
-        <v>155</v>
-      </c>
       <c r="I29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="150" x14ac:dyDescent="0.25">
@@ -3668,28 +3667,28 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C30" t="s">
         <v>156</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D30" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" t="s">
-        <v>12</v>
-      </c>
-      <c r="F30" s="1" t="s">
+      <c r="G30" t="s">
         <v>158</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>159</v>
       </c>
-      <c r="H30" t="s">
-        <v>160</v>
-      </c>
       <c r="I30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="285" x14ac:dyDescent="0.25">
@@ -3697,28 +3696,28 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C31" t="s">
         <v>161</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" t="s">
+        <v>55</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="G31" t="s">
         <v>162</v>
       </c>
-      <c r="D31" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31" t="s">
-        <v>56</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>610</v>
-      </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>163</v>
       </c>
-      <c r="H31" t="s">
-        <v>164</v>
-      </c>
       <c r="I31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="180" x14ac:dyDescent="0.25">
@@ -3726,28 +3725,28 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C32" t="s">
         <v>165</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" t="s">
+        <v>55</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="G32" t="s">
         <v>166</v>
       </c>
-      <c r="D32" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32" t="s">
-        <v>56</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>642</v>
-      </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>167</v>
       </c>
-      <c r="H32" t="s">
-        <v>168</v>
-      </c>
       <c r="I32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -3755,28 +3754,28 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C33" t="s">
+        <v>161</v>
+      </c>
+      <c r="D33" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" t="s">
+        <v>55</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="C33" t="s">
-        <v>162</v>
-      </c>
-      <c r="D33" t="s">
-        <v>11</v>
-      </c>
-      <c r="E33" t="s">
-        <v>56</v>
-      </c>
-      <c r="F33" s="1" t="s">
+      <c r="G33" t="s">
         <v>170</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>171</v>
       </c>
-      <c r="H33" t="s">
-        <v>172</v>
-      </c>
       <c r="I33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="180" x14ac:dyDescent="0.25">
@@ -3784,28 +3783,28 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C34" t="s">
+        <v>161</v>
+      </c>
+      <c r="D34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" t="s">
+        <v>55</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C34" t="s">
-        <v>162</v>
-      </c>
-      <c r="D34" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34" t="s">
-        <v>56</v>
-      </c>
-      <c r="F34" s="1" t="s">
+      <c r="G34" t="s">
         <v>174</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>175</v>
       </c>
-      <c r="H34" t="s">
-        <v>176</v>
-      </c>
       <c r="I34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="105" x14ac:dyDescent="0.25">
@@ -3813,28 +3812,28 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C35" t="s">
         <v>177</v>
-      </c>
-      <c r="C35" t="s">
-        <v>178</v>
       </c>
       <c r="D35">
         <v>1994</v>
       </c>
       <c r="E35" t="s">
+        <v>178</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="G35" t="s">
         <v>180</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>181</v>
       </c>
-      <c r="H35" t="s">
-        <v>182</v>
-      </c>
       <c r="I35" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="225" x14ac:dyDescent="0.25">
@@ -3842,28 +3841,28 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C36" t="s">
         <v>183</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="G36" t="s">
         <v>184</v>
       </c>
-      <c r="D36" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36" t="s">
-        <v>11</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>611</v>
-      </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>185</v>
       </c>
-      <c r="H36" t="s">
-        <v>186</v>
-      </c>
       <c r="I36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -3871,28 +3870,28 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C37" t="s">
         <v>187</v>
-      </c>
-      <c r="C37" t="s">
-        <v>188</v>
       </c>
       <c r="D37">
         <v>1948</v>
       </c>
       <c r="E37" t="s">
+        <v>188</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="G37" t="s">
         <v>190</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>191</v>
       </c>
-      <c r="H37" t="s">
-        <v>192</v>
-      </c>
       <c r="I37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -3900,28 +3899,28 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C38" t="s">
         <v>193</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="D38" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" t="s">
-        <v>11</v>
-      </c>
-      <c r="F38" s="1" t="s">
+      <c r="G38" t="s">
         <v>195</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H38" t="s">
         <v>196</v>
       </c>
-      <c r="H38" t="s">
-        <v>197</v>
-      </c>
       <c r="I38" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -3929,28 +3928,28 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C39" t="s">
         <v>198</v>
-      </c>
-      <c r="C39" t="s">
-        <v>199</v>
       </c>
       <c r="D39">
         <v>1995</v>
       </c>
       <c r="E39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F39" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="G39" t="s">
         <v>200</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>201</v>
       </c>
-      <c r="H39" t="s">
-        <v>202</v>
-      </c>
       <c r="I39" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3958,28 +3957,28 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C40" t="s">
         <v>203</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="D40" t="s">
-        <v>11</v>
-      </c>
-      <c r="E40" t="s">
-        <v>12</v>
-      </c>
-      <c r="F40" s="1" t="s">
+      <c r="G40" t="s">
         <v>205</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>206</v>
       </c>
-      <c r="H40" t="s">
-        <v>207</v>
-      </c>
       <c r="I40" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -3987,28 +3986,28 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C41" t="s">
         <v>208</v>
-      </c>
-      <c r="C41" t="s">
-        <v>209</v>
       </c>
       <c r="D41">
         <v>1995</v>
       </c>
       <c r="E41" t="s">
+        <v>209</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="G41" t="s">
         <v>211</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>212</v>
       </c>
-      <c r="H41" t="s">
-        <v>213</v>
-      </c>
       <c r="I41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -4016,28 +4015,28 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C42" t="s">
         <v>214</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" t="s">
         <v>215</v>
       </c>
-      <c r="D42" t="s">
-        <v>11</v>
-      </c>
-      <c r="E42" t="s">
+      <c r="F42" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="G42" t="s">
         <v>217</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>218</v>
       </c>
-      <c r="H42" t="s">
-        <v>219</v>
-      </c>
       <c r="I42" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -4045,28 +4044,28 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C43" t="s">
         <v>220</v>
-      </c>
-      <c r="C43" t="s">
-        <v>221</v>
       </c>
       <c r="D43">
         <v>2003</v>
       </c>
       <c r="E43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F43" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G43" t="s">
         <v>222</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H43" t="s">
         <v>223</v>
       </c>
-      <c r="H43" t="s">
-        <v>224</v>
-      </c>
       <c r="I43" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="180" x14ac:dyDescent="0.25">
@@ -4074,28 +4073,28 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C44" t="s">
         <v>225</v>
-      </c>
-      <c r="C44" t="s">
-        <v>226</v>
       </c>
       <c r="D44">
         <v>1993</v>
       </c>
       <c r="E44" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="G44" t="s">
+        <v>226</v>
+      </c>
+      <c r="H44" t="s">
         <v>227</v>
       </c>
-      <c r="H44" t="s">
+      <c r="I44" t="s">
         <v>228</v>
-      </c>
-      <c r="I44" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -4103,28 +4102,28 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C45" t="s">
         <v>230</v>
-      </c>
-      <c r="C45" t="s">
-        <v>231</v>
       </c>
       <c r="D45">
         <v>2002</v>
       </c>
       <c r="E45" t="s">
+        <v>231</v>
+      </c>
+      <c r="F45" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="G45" t="s">
         <v>233</v>
       </c>
-      <c r="G45" t="s">
+      <c r="H45" t="s">
         <v>234</v>
       </c>
-      <c r="H45" t="s">
-        <v>235</v>
-      </c>
       <c r="I45" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="195" x14ac:dyDescent="0.25">
@@ -4132,28 +4131,28 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C46" t="s">
         <v>236</v>
-      </c>
-      <c r="C46" t="s">
-        <v>237</v>
       </c>
       <c r="D46">
         <v>2004</v>
       </c>
       <c r="E46" t="s">
+        <v>237</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="G46" t="s">
         <v>238</v>
       </c>
-      <c r="F46" s="1" t="s">
-        <v>613</v>
-      </c>
-      <c r="G46" t="s">
+      <c r="H46" t="s">
         <v>239</v>
       </c>
-      <c r="H46" t="s">
-        <v>240</v>
-      </c>
       <c r="I46" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -4161,28 +4160,28 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C47" t="s">
         <v>241</v>
-      </c>
-      <c r="C47" t="s">
-        <v>242</v>
       </c>
       <c r="D47">
         <v>2001</v>
       </c>
       <c r="E47" t="s">
+        <v>242</v>
+      </c>
+      <c r="F47" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="G47" t="s">
         <v>244</v>
       </c>
-      <c r="G47" t="s">
+      <c r="H47" t="s">
         <v>245</v>
       </c>
-      <c r="H47" t="s">
-        <v>246</v>
-      </c>
       <c r="I47" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -4190,28 +4189,28 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C48" t="s">
         <v>247</v>
-      </c>
-      <c r="C48" t="s">
-        <v>248</v>
       </c>
       <c r="D48">
         <v>1978</v>
       </c>
       <c r="E48" t="s">
+        <v>248</v>
+      </c>
+      <c r="F48" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="G48" t="s">
         <v>250</v>
       </c>
-      <c r="G48" t="s">
+      <c r="H48" t="s">
         <v>251</v>
       </c>
-      <c r="H48" t="s">
-        <v>252</v>
-      </c>
       <c r="I48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -4219,28 +4218,28 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C49" t="s">
         <v>253</v>
-      </c>
-      <c r="C49" t="s">
-        <v>254</v>
       </c>
       <c r="D49">
         <v>2005</v>
       </c>
       <c r="E49" t="s">
+        <v>254</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="G49" t="s">
         <v>256</v>
       </c>
-      <c r="G49" t="s">
+      <c r="H49" t="s">
         <v>257</v>
       </c>
-      <c r="H49" t="s">
-        <v>258</v>
-      </c>
       <c r="I49" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="135" x14ac:dyDescent="0.25">
@@ -4248,28 +4247,28 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C50" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D50">
         <v>2003</v>
       </c>
       <c r="E50" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="G50" t="s">
+        <v>259</v>
+      </c>
+      <c r="H50" t="s">
         <v>260</v>
       </c>
-      <c r="H50" t="s">
-        <v>261</v>
-      </c>
       <c r="I50" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="150" x14ac:dyDescent="0.25">
@@ -4277,28 +4276,28 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C51" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D51">
         <v>2003</v>
       </c>
       <c r="E51" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="G51" t="s">
+        <v>262</v>
+      </c>
+      <c r="H51" t="s">
         <v>263</v>
       </c>
-      <c r="H51" t="s">
-        <v>264</v>
-      </c>
       <c r="I51" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="195" x14ac:dyDescent="0.25">
@@ -4306,28 +4305,28 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C52" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D52">
         <v>2003</v>
       </c>
       <c r="E52" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="G52" t="s">
+        <v>265</v>
+      </c>
+      <c r="H52" t="s">
         <v>266</v>
       </c>
-      <c r="H52" t="s">
-        <v>267</v>
-      </c>
       <c r="I52" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="135" x14ac:dyDescent="0.25">
@@ -4335,28 +4334,28 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C53" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D53">
         <v>2003</v>
       </c>
       <c r="E53" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F53" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="G53" t="s">
         <v>269</v>
       </c>
-      <c r="G53" t="s">
+      <c r="H53" t="s">
         <v>270</v>
       </c>
-      <c r="H53" t="s">
-        <v>271</v>
-      </c>
       <c r="I53" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -4364,28 +4363,28 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C54" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D54">
         <v>2003</v>
       </c>
       <c r="E54" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F54" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="G54" t="s">
         <v>273</v>
       </c>
-      <c r="G54" t="s">
+      <c r="H54" t="s">
         <v>274</v>
       </c>
-      <c r="H54" t="s">
-        <v>275</v>
-      </c>
       <c r="I54" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4393,28 +4392,28 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C55" t="s">
         <v>276</v>
-      </c>
-      <c r="C55" t="s">
-        <v>277</v>
       </c>
       <c r="D55">
         <v>1966</v>
       </c>
       <c r="E55" t="s">
+        <v>277</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G55" t="s">
         <v>278</v>
       </c>
-      <c r="F55" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G55" t="s">
+      <c r="H55" t="s">
         <v>279</v>
       </c>
-      <c r="H55" t="s">
-        <v>280</v>
-      </c>
       <c r="I55" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4422,28 +4421,28 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C56" t="s">
         <v>281</v>
-      </c>
-      <c r="C56" t="s">
-        <v>282</v>
       </c>
       <c r="D56">
         <v>1996</v>
       </c>
       <c r="E56" t="s">
+        <v>282</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="F56" s="1" t="s">
+      <c r="G56" t="s">
         <v>284</v>
       </c>
-      <c r="G56" t="s">
+      <c r="H56" t="s">
         <v>285</v>
       </c>
-      <c r="H56" t="s">
-        <v>286</v>
-      </c>
       <c r="I56" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -4451,28 +4450,28 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C57" t="s">
         <v>287</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
+        <v>10</v>
+      </c>
+      <c r="E57" t="s">
+        <v>11</v>
+      </c>
+      <c r="F57" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="D57" t="s">
-        <v>11</v>
-      </c>
-      <c r="E57" t="s">
-        <v>12</v>
-      </c>
-      <c r="F57" s="1" t="s">
+      <c r="G57" t="s">
         <v>289</v>
       </c>
-      <c r="G57" t="s">
+      <c r="H57" t="s">
         <v>290</v>
       </c>
-      <c r="H57" t="s">
-        <v>291</v>
-      </c>
       <c r="I57" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4480,28 +4479,28 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C58" t="s">
+        <v>31</v>
+      </c>
+      <c r="D58" t="s">
+        <v>10</v>
+      </c>
+      <c r="E58" t="s">
         <v>292</v>
       </c>
-      <c r="C58" t="s">
-        <v>32</v>
-      </c>
-      <c r="D58" t="s">
-        <v>11</v>
-      </c>
-      <c r="E58" t="s">
+      <c r="F58" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="F58" s="1" t="s">
+      <c r="G58" t="s">
         <v>294</v>
       </c>
-      <c r="G58" t="s">
+      <c r="H58" t="s">
         <v>295</v>
       </c>
-      <c r="H58" t="s">
-        <v>296</v>
-      </c>
       <c r="I58" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="150" x14ac:dyDescent="0.25">
@@ -4509,28 +4508,28 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C59" t="s">
         <v>297</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
+        <v>10</v>
+      </c>
+      <c r="E59" t="s">
         <v>298</v>
       </c>
-      <c r="D59" t="s">
-        <v>11</v>
-      </c>
-      <c r="E59" t="s">
+      <c r="F59" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="F59" s="1" t="s">
+      <c r="G59" t="s">
         <v>300</v>
       </c>
-      <c r="G59" t="s">
+      <c r="H59" t="s">
         <v>301</v>
       </c>
-      <c r="H59" t="s">
-        <v>302</v>
-      </c>
       <c r="I59" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="195" x14ac:dyDescent="0.25">
@@ -4538,28 +4537,28 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C60" t="s">
         <v>303</v>
-      </c>
-      <c r="C60" t="s">
-        <v>304</v>
       </c>
       <c r="D60">
         <v>2000</v>
       </c>
       <c r="E60" t="s">
+        <v>304</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="G60" t="s">
         <v>305</v>
       </c>
-      <c r="F60" s="1" t="s">
-        <v>617</v>
-      </c>
-      <c r="G60" t="s">
+      <c r="H60" t="s">
         <v>306</v>
       </c>
-      <c r="H60" t="s">
-        <v>307</v>
-      </c>
       <c r="I60" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="210" x14ac:dyDescent="0.25">
@@ -4567,28 +4566,28 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C61" t="s">
+        <v>161</v>
+      </c>
+      <c r="D61" t="s">
+        <v>10</v>
+      </c>
+      <c r="E61" t="s">
+        <v>55</v>
+      </c>
+      <c r="F61" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="C61" t="s">
-        <v>162</v>
-      </c>
-      <c r="D61" t="s">
-        <v>11</v>
-      </c>
-      <c r="E61" t="s">
-        <v>56</v>
-      </c>
-      <c r="F61" s="1" t="s">
+      <c r="G61" t="s">
         <v>309</v>
       </c>
-      <c r="G61" t="s">
+      <c r="H61" t="s">
         <v>310</v>
       </c>
-      <c r="H61" t="s">
-        <v>311</v>
-      </c>
       <c r="I61" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="135" x14ac:dyDescent="0.25">
@@ -4596,28 +4595,28 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C62" t="s">
         <v>312</v>
-      </c>
-      <c r="C62" t="s">
-        <v>313</v>
       </c>
       <c r="D62">
         <v>2009</v>
       </c>
       <c r="E62" t="s">
+        <v>313</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="G62" t="s">
         <v>314</v>
       </c>
-      <c r="F62" s="1" t="s">
-        <v>618</v>
-      </c>
-      <c r="G62" t="s">
+      <c r="H62" t="s">
         <v>315</v>
       </c>
-      <c r="H62" t="s">
-        <v>316</v>
-      </c>
       <c r="I62" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -4625,28 +4624,28 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C63" t="s">
+        <v>152</v>
+      </c>
+      <c r="D63" t="s">
+        <v>10</v>
+      </c>
+      <c r="E63" t="s">
+        <v>55</v>
+      </c>
+      <c r="F63" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="C63" t="s">
-        <v>153</v>
-      </c>
-      <c r="D63" t="s">
-        <v>11</v>
-      </c>
-      <c r="E63" t="s">
-        <v>56</v>
-      </c>
-      <c r="F63" s="1" t="s">
+      <c r="G63" t="s">
         <v>318</v>
       </c>
-      <c r="G63" t="s">
+      <c r="H63" t="s">
         <v>319</v>
       </c>
-      <c r="H63" t="s">
-        <v>320</v>
-      </c>
       <c r="I63" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -4654,28 +4653,28 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C64" t="s">
         <v>321</v>
-      </c>
-      <c r="C64" t="s">
-        <v>322</v>
       </c>
       <c r="D64">
         <v>2004</v>
       </c>
       <c r="E64" t="s">
+        <v>322</v>
+      </c>
+      <c r="F64" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="F64" s="1" t="s">
+      <c r="G64" t="s">
         <v>324</v>
       </c>
-      <c r="G64" t="s">
+      <c r="H64" t="s">
         <v>325</v>
       </c>
-      <c r="H64" t="s">
-        <v>326</v>
-      </c>
       <c r="I64" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="105" x14ac:dyDescent="0.25">
@@ -4683,28 +4682,28 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C65" t="s">
         <v>327</v>
-      </c>
-      <c r="C65" t="s">
-        <v>328</v>
       </c>
       <c r="D65">
         <v>2002</v>
       </c>
       <c r="E65" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F65" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="G65" t="s">
         <v>329</v>
       </c>
-      <c r="G65" t="s">
+      <c r="H65" t="s">
         <v>330</v>
       </c>
-      <c r="H65" t="s">
-        <v>331</v>
-      </c>
       <c r="I65" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -4712,28 +4711,28 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C66" t="s">
+        <v>10</v>
+      </c>
+      <c r="D66" t="s">
+        <v>10</v>
+      </c>
+      <c r="E66" t="s">
+        <v>10</v>
+      </c>
+      <c r="F66" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="C66" t="s">
-        <v>11</v>
-      </c>
-      <c r="D66" t="s">
-        <v>11</v>
-      </c>
-      <c r="E66" t="s">
-        <v>11</v>
-      </c>
-      <c r="F66" s="1" t="s">
+      <c r="G66" t="s">
         <v>333</v>
       </c>
-      <c r="G66" t="s">
+      <c r="H66" t="s">
         <v>334</v>
       </c>
-      <c r="H66" t="s">
-        <v>335</v>
-      </c>
       <c r="I66" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -4741,28 +4740,28 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C67" t="s">
         <v>336</v>
-      </c>
-      <c r="C67" t="s">
-        <v>337</v>
       </c>
       <c r="D67">
         <v>1964</v>
       </c>
       <c r="E67" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F67" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="G67" t="s">
         <v>338</v>
       </c>
-      <c r="G67" t="s">
+      <c r="H67" t="s">
         <v>339</v>
       </c>
-      <c r="H67" t="s">
-        <v>340</v>
-      </c>
       <c r="I67" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -4770,28 +4769,28 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="C68" t="s">
         <v>341</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D68" t="s">
+        <v>10</v>
+      </c>
+      <c r="E68" t="s">
+        <v>11</v>
+      </c>
+      <c r="F68" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="D68" t="s">
-        <v>11</v>
-      </c>
-      <c r="E68" t="s">
-        <v>12</v>
-      </c>
-      <c r="F68" s="1" t="s">
+      <c r="G68" t="s">
         <v>343</v>
       </c>
-      <c r="G68" t="s">
+      <c r="H68" t="s">
         <v>344</v>
       </c>
-      <c r="H68" t="s">
-        <v>345</v>
-      </c>
       <c r="I68" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4799,28 +4798,28 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="C69" t="s">
         <v>346</v>
       </c>
-      <c r="C69" t="s">
+      <c r="D69" t="s">
+        <v>10</v>
+      </c>
+      <c r="E69" t="s">
+        <v>11</v>
+      </c>
+      <c r="F69" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="D69" t="s">
-        <v>11</v>
-      </c>
-      <c r="E69" t="s">
-        <v>12</v>
-      </c>
-      <c r="F69" s="1" t="s">
+      <c r="G69" t="s">
         <v>348</v>
       </c>
-      <c r="G69" t="s">
+      <c r="H69" t="s">
         <v>349</v>
       </c>
-      <c r="H69" t="s">
-        <v>350</v>
-      </c>
       <c r="I69" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -4828,28 +4827,28 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C70" t="s">
         <v>351</v>
-      </c>
-      <c r="C70" t="s">
-        <v>352</v>
       </c>
       <c r="D70">
         <v>2002</v>
       </c>
       <c r="E70" t="s">
+        <v>352</v>
+      </c>
+      <c r="F70" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="F70" s="1" t="s">
+      <c r="G70" t="s">
         <v>354</v>
       </c>
-      <c r="G70" t="s">
+      <c r="H70" t="s">
         <v>355</v>
       </c>
-      <c r="H70" t="s">
+      <c r="I70" t="s">
         <v>356</v>
-      </c>
-      <c r="I70" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -4857,28 +4856,28 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C71" t="s">
         <v>358</v>
-      </c>
-      <c r="C71" t="s">
-        <v>359</v>
       </c>
       <c r="D71">
         <v>2011</v>
       </c>
       <c r="E71" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="G71" t="s">
+        <v>359</v>
+      </c>
+      <c r="H71" t="s">
         <v>360</v>
       </c>
-      <c r="H71" t="s">
-        <v>361</v>
-      </c>
       <c r="I71" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -4886,28 +4885,28 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C72" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D72">
         <v>1998</v>
       </c>
       <c r="E72" t="s">
+        <v>362</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="G72" t="s">
         <v>363</v>
       </c>
-      <c r="F72" s="1" t="s">
-        <v>620</v>
-      </c>
-      <c r="G72" t="s">
+      <c r="H72" t="s">
         <v>364</v>
       </c>
-      <c r="H72" t="s">
-        <v>365</v>
-      </c>
       <c r="I72" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4915,28 +4914,28 @@
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="C73" t="s">
         <v>366</v>
-      </c>
-      <c r="C73" t="s">
-        <v>367</v>
       </c>
       <c r="D73">
         <v>2000</v>
       </c>
       <c r="E73" t="s">
+        <v>367</v>
+      </c>
+      <c r="F73" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="F73" s="1" t="s">
+      <c r="G73" t="s">
         <v>369</v>
       </c>
-      <c r="G73" t="s">
+      <c r="H73" t="s">
         <v>370</v>
       </c>
-      <c r="H73" t="s">
-        <v>371</v>
-      </c>
       <c r="I73" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -4944,28 +4943,28 @@
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="C74" t="s">
         <v>372</v>
-      </c>
-      <c r="C74" t="s">
-        <v>373</v>
       </c>
       <c r="D74">
         <v>2004</v>
       </c>
       <c r="E74" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F74" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="G74" t="s">
         <v>374</v>
       </c>
-      <c r="G74" t="s">
+      <c r="H74" t="s">
         <v>375</v>
       </c>
-      <c r="H74" t="s">
+      <c r="I74" t="s">
         <v>376</v>
-      </c>
-      <c r="I74" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -4973,28 +4972,28 @@
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C75" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D75">
         <v>2006</v>
       </c>
       <c r="E75" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F75" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="G75" t="s">
         <v>379</v>
       </c>
-      <c r="G75" t="s">
+      <c r="H75" t="s">
         <v>380</v>
       </c>
-      <c r="H75" t="s">
-        <v>381</v>
-      </c>
       <c r="I75" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -5002,28 +5001,28 @@
         <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C76" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D76">
         <v>2011</v>
       </c>
       <c r="E76" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F76" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="G76" t="s">
         <v>383</v>
       </c>
-      <c r="G76" t="s">
+      <c r="H76" t="s">
         <v>384</v>
       </c>
-      <c r="H76" t="s">
-        <v>385</v>
-      </c>
       <c r="I76" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="105" x14ac:dyDescent="0.25">
@@ -5031,28 +5030,28 @@
         <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C77" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D77">
         <v>2010</v>
       </c>
       <c r="E77" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F77" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="G77" t="s">
         <v>387</v>
       </c>
-      <c r="G77" t="s">
+      <c r="H77" t="s">
         <v>388</v>
       </c>
-      <c r="H77" t="s">
-        <v>389</v>
-      </c>
       <c r="I77" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -5060,28 +5059,28 @@
         <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C78" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D78">
         <v>2010</v>
       </c>
       <c r="E78" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F78" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="G78" t="s">
         <v>391</v>
       </c>
-      <c r="G78" t="s">
+      <c r="H78" t="s">
         <v>392</v>
       </c>
-      <c r="H78" t="s">
-        <v>393</v>
-      </c>
       <c r="I78" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -5089,28 +5088,28 @@
         <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C79" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D79">
         <v>2011</v>
       </c>
       <c r="E79" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F79" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="G79" t="s">
         <v>395</v>
       </c>
-      <c r="G79" t="s">
+      <c r="H79" t="s">
         <v>396</v>
       </c>
-      <c r="H79" t="s">
-        <v>397</v>
-      </c>
       <c r="I79" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -5118,28 +5117,28 @@
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C80" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D80">
         <v>2011</v>
       </c>
       <c r="E80" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F80" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="G80" t="s">
         <v>399</v>
       </c>
-      <c r="G80" t="s">
+      <c r="H80" t="s">
         <v>400</v>
       </c>
-      <c r="H80" t="s">
-        <v>401</v>
-      </c>
       <c r="I80" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -5147,28 +5146,28 @@
         <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C81" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D81">
         <v>2003</v>
       </c>
       <c r="E81" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F81" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="G81" t="s">
         <v>403</v>
       </c>
-      <c r="G81" t="s">
+      <c r="H81" t="s">
         <v>404</v>
       </c>
-      <c r="H81" t="s">
-        <v>405</v>
-      </c>
       <c r="I81" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -5176,28 +5175,28 @@
         <v>81</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C82" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D82">
         <v>2004</v>
       </c>
       <c r="E82" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F82" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="G82" t="s">
         <v>407</v>
       </c>
-      <c r="G82" t="s">
+      <c r="H82" t="s">
         <v>408</v>
       </c>
-      <c r="H82" t="s">
-        <v>409</v>
-      </c>
       <c r="I82" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
@@ -5205,28 +5204,28 @@
         <v>82</v>
       </c>
       <c r="B83" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C83" t="s">
         <v>410</v>
       </c>
-      <c r="C83" t="s">
+      <c r="D83" t="s">
+        <v>10</v>
+      </c>
+      <c r="E83" t="s">
+        <v>124</v>
+      </c>
+      <c r="F83" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="D83" t="s">
-        <v>11</v>
-      </c>
-      <c r="E83" t="s">
-        <v>125</v>
-      </c>
-      <c r="F83" s="1" t="s">
+      <c r="G83" t="s">
         <v>412</v>
       </c>
-      <c r="G83" t="s">
+      <c r="H83" t="s">
         <v>413</v>
       </c>
-      <c r="H83" t="s">
-        <v>414</v>
-      </c>
       <c r="I83" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5234,28 +5233,28 @@
         <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C84" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D84">
         <v>2001</v>
       </c>
       <c r="E84" t="s">
+        <v>415</v>
+      </c>
+      <c r="F84" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="F84" s="1" t="s">
+      <c r="G84" t="s">
         <v>417</v>
       </c>
-      <c r="G84" t="s">
+      <c r="H84" t="s">
         <v>418</v>
       </c>
-      <c r="H84" t="s">
-        <v>419</v>
-      </c>
       <c r="I84" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -5263,28 +5262,28 @@
         <v>84</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C85" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D85">
         <v>2001</v>
       </c>
       <c r="E85" t="s">
+        <v>420</v>
+      </c>
+      <c r="F85" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="F85" s="1" t="s">
+      <c r="G85" t="s">
         <v>422</v>
       </c>
-      <c r="G85" t="s">
+      <c r="H85" t="s">
         <v>423</v>
       </c>
-      <c r="H85" t="s">
-        <v>424</v>
-      </c>
       <c r="I85" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -5292,28 +5291,28 @@
         <v>85</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C86" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D86">
         <v>2001</v>
       </c>
       <c r="E86" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F86" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="G86" t="s">
         <v>426</v>
       </c>
-      <c r="G86" t="s">
+      <c r="H86" t="s">
         <v>427</v>
       </c>
-      <c r="H86" t="s">
-        <v>428</v>
-      </c>
       <c r="I86" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -5321,28 +5320,28 @@
         <v>86</v>
       </c>
       <c r="B87" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="C87" t="s">
         <v>429</v>
-      </c>
-      <c r="C87" t="s">
-        <v>430</v>
       </c>
       <c r="D87">
         <v>2005</v>
       </c>
       <c r="E87" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F87" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="G87" t="s">
         <v>431</v>
       </c>
-      <c r="G87" t="s">
+      <c r="H87" t="s">
         <v>432</v>
       </c>
-      <c r="H87" t="s">
-        <v>433</v>
-      </c>
       <c r="I87" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5350,28 +5349,28 @@
         <v>87</v>
       </c>
       <c r="B88" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="C88" t="s">
         <v>434</v>
-      </c>
-      <c r="C88" t="s">
-        <v>435</v>
       </c>
       <c r="D88">
         <v>2009</v>
       </c>
       <c r="E88" t="s">
+        <v>435</v>
+      </c>
+      <c r="F88" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="F88" s="1" t="s">
+      <c r="G88" t="s">
         <v>437</v>
       </c>
-      <c r="G88" t="s">
+      <c r="H88" t="s">
         <v>438</v>
       </c>
-      <c r="H88" t="s">
-        <v>439</v>
-      </c>
       <c r="I88" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="375" x14ac:dyDescent="0.25">
@@ -5379,28 +5378,28 @@
         <v>88</v>
       </c>
       <c r="B89" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="C89" t="s">
         <v>440</v>
-      </c>
-      <c r="C89" t="s">
-        <v>441</v>
       </c>
       <c r="D89">
         <v>1999</v>
       </c>
       <c r="E89" t="s">
+        <v>441</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="G89" t="s">
         <v>442</v>
       </c>
-      <c r="F89" s="1" t="s">
-        <v>621</v>
-      </c>
-      <c r="G89" t="s">
+      <c r="H89" t="s">
         <v>443</v>
       </c>
-      <c r="H89" t="s">
-        <v>444</v>
-      </c>
       <c r="I89" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="135" x14ac:dyDescent="0.25">
@@ -5408,28 +5407,28 @@
         <v>89</v>
       </c>
       <c r="B90" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="C90" t="s">
         <v>445</v>
-      </c>
-      <c r="C90" t="s">
-        <v>446</v>
       </c>
       <c r="D90">
         <v>1973</v>
       </c>
       <c r="E90" t="s">
+        <v>446</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="G90" t="s">
         <v>447</v>
       </c>
-      <c r="F90" s="1" t="s">
-        <v>643</v>
-      </c>
-      <c r="G90" t="s">
+      <c r="H90" t="s">
         <v>448</v>
       </c>
-      <c r="H90" t="s">
-        <v>449</v>
-      </c>
       <c r="I90" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -5437,28 +5436,28 @@
         <v>90</v>
       </c>
       <c r="B91" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="C91" t="s">
         <v>450</v>
-      </c>
-      <c r="C91" t="s">
-        <v>451</v>
       </c>
       <c r="D91">
         <v>2006</v>
       </c>
       <c r="E91" t="s">
+        <v>451</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="G91" t="s">
         <v>452</v>
       </c>
-      <c r="F91" s="1" t="s">
-        <v>644</v>
-      </c>
-      <c r="G91" t="s">
+      <c r="H91" t="s">
         <v>453</v>
       </c>
-      <c r="H91" t="s">
-        <v>454</v>
-      </c>
       <c r="I91" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -5466,28 +5465,28 @@
         <v>91</v>
       </c>
       <c r="B92" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="C92" t="s">
         <v>455</v>
       </c>
-      <c r="C92" t="s">
+      <c r="D92" t="s">
+        <v>10</v>
+      </c>
+      <c r="E92" t="s">
         <v>456</v>
       </c>
-      <c r="D92" t="s">
-        <v>11</v>
-      </c>
-      <c r="E92" t="s">
+      <c r="F92" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="G92" t="s">
         <v>457</v>
       </c>
-      <c r="F92" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="G92" t="s">
+      <c r="H92" t="s">
         <v>458</v>
       </c>
-      <c r="H92" t="s">
-        <v>459</v>
-      </c>
       <c r="I92" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="93" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -5495,28 +5494,28 @@
         <v>92</v>
       </c>
       <c r="B93" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="C93" t="s">
         <v>460</v>
       </c>
-      <c r="C93" t="s">
-        <v>461</v>
-      </c>
       <c r="D93" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E93" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G93" t="s">
+        <v>462</v>
+      </c>
+      <c r="H93" t="s">
         <v>463</v>
       </c>
-      <c r="H93" t="s">
-        <v>464</v>
-      </c>
       <c r="I93" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="225" x14ac:dyDescent="0.25">
@@ -5524,28 +5523,28 @@
         <v>93</v>
       </c>
       <c r="B94" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="C94" t="s">
         <v>465</v>
       </c>
-      <c r="C94" t="s">
-        <v>466</v>
-      </c>
       <c r="D94" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E94" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="G94" t="s">
+        <v>467</v>
+      </c>
+      <c r="H94" t="s">
         <v>468</v>
       </c>
-      <c r="H94" t="s">
-        <v>469</v>
-      </c>
       <c r="I94" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -5553,28 +5552,28 @@
         <v>94</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C95" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D95">
         <v>2003</v>
       </c>
       <c r="E95" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G95" t="s">
+        <v>470</v>
+      </c>
+      <c r="H95" t="s">
         <v>471</v>
       </c>
-      <c r="H95" t="s">
-        <v>472</v>
-      </c>
       <c r="I95" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="96" spans="1:9" ht="150" x14ac:dyDescent="0.25">
@@ -5582,28 +5581,28 @@
         <v>95</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C96" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D96">
         <v>2002</v>
       </c>
       <c r="E96" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G96" t="s">
+        <v>474</v>
+      </c>
+      <c r="H96" t="s">
         <v>475</v>
       </c>
-      <c r="H96" t="s">
-        <v>476</v>
-      </c>
       <c r="I96" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="97" spans="1:10" ht="135" x14ac:dyDescent="0.25">
@@ -5611,28 +5610,28 @@
         <v>96</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C97" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D97">
         <v>2003</v>
       </c>
       <c r="E97" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G97" t="s">
+        <v>477</v>
+      </c>
+      <c r="H97" t="s">
         <v>478</v>
       </c>
-      <c r="H97" t="s">
-        <v>479</v>
-      </c>
       <c r="I97" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="98" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -5640,28 +5639,28 @@
         <v>97</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C98" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D98">
         <v>2002</v>
       </c>
       <c r="E98" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="G98" t="s">
+        <v>481</v>
+      </c>
+      <c r="H98" t="s">
         <v>482</v>
       </c>
-      <c r="H98" t="s">
-        <v>483</v>
-      </c>
       <c r="I98" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="99" spans="1:10" ht="195" x14ac:dyDescent="0.25">
@@ -5669,28 +5668,28 @@
         <v>98</v>
       </c>
       <c r="B99" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="C99" t="s">
         <v>484</v>
-      </c>
-      <c r="C99" t="s">
-        <v>485</v>
       </c>
       <c r="D99">
         <v>2002</v>
       </c>
       <c r="E99" t="s">
+        <v>485</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="G99" t="s">
         <v>486</v>
       </c>
-      <c r="F99" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="G99" t="s">
+      <c r="H99" t="s">
         <v>487</v>
       </c>
-      <c r="H99" t="s">
-        <v>488</v>
-      </c>
       <c r="I99" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="100" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -5698,28 +5697,28 @@
         <v>99</v>
       </c>
       <c r="B100" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="C100" t="s">
         <v>489</v>
-      </c>
-      <c r="C100" t="s">
-        <v>490</v>
       </c>
       <c r="D100">
         <v>2006</v>
       </c>
       <c r="E100" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="G100" t="s">
+        <v>491</v>
+      </c>
+      <c r="H100" t="s">
         <v>492</v>
       </c>
-      <c r="H100" t="s">
-        <v>493</v>
-      </c>
       <c r="I100" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="101" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -5727,31 +5726,31 @@
         <v>100</v>
       </c>
       <c r="B101" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="C101" t="s">
         <v>494</v>
-      </c>
-      <c r="C101" t="s">
-        <v>495</v>
       </c>
       <c r="D101">
         <v>2018</v>
       </c>
       <c r="E101" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="G101" t="s">
+        <v>497</v>
+      </c>
+      <c r="H101" t="s">
         <v>498</v>
       </c>
-      <c r="H101" t="s">
+      <c r="I101" t="s">
         <v>499</v>
       </c>
-      <c r="I101" t="s">
+      <c r="J101" t="s">
         <v>500</v>
-      </c>
-      <c r="J101" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="102" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -5759,31 +5758,31 @@
         <v>101</v>
       </c>
       <c r="B102" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="C102" t="s">
         <v>502</v>
-      </c>
-      <c r="C102" t="s">
-        <v>503</v>
       </c>
       <c r="D102">
         <v>2018</v>
       </c>
       <c r="E102" t="s">
+        <v>503</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="G102" t="s">
         <v>504</v>
       </c>
-      <c r="F102" s="1" t="s">
-        <v>625</v>
-      </c>
-      <c r="G102" t="s">
+      <c r="H102" t="s">
         <v>505</v>
       </c>
-      <c r="H102" t="s">
+      <c r="I102" t="s">
+        <v>66</v>
+      </c>
+      <c r="J102" t="s">
         <v>506</v>
-      </c>
-      <c r="I102" t="s">
-        <v>67</v>
-      </c>
-      <c r="J102" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="103" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -5791,31 +5790,31 @@
         <v>102</v>
       </c>
       <c r="B103" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="C103" t="s">
         <v>508</v>
-      </c>
-      <c r="C103" t="s">
-        <v>509</v>
       </c>
       <c r="D103">
         <v>2018</v>
       </c>
       <c r="E103" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="G103" t="s">
+        <v>509</v>
+      </c>
+      <c r="H103" t="s">
         <v>510</v>
       </c>
-      <c r="H103" t="s">
+      <c r="I103" t="s">
+        <v>52</v>
+      </c>
+      <c r="J103" t="s">
         <v>511</v>
-      </c>
-      <c r="I103" t="s">
-        <v>53</v>
-      </c>
-      <c r="J103" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="104" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -5823,28 +5822,28 @@
         <v>103</v>
       </c>
       <c r="B104" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="C104" t="s">
         <v>513</v>
-      </c>
-      <c r="C104" t="s">
-        <v>514</v>
       </c>
       <c r="D104">
         <v>2018</v>
       </c>
       <c r="E104" t="s">
+        <v>514</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="G104" t="s">
         <v>515</v>
       </c>
-      <c r="F104" s="1" t="s">
-        <v>627</v>
-      </c>
-      <c r="G104" t="s">
+      <c r="H104" t="s">
         <v>516</v>
       </c>
-      <c r="H104" t="s">
-        <v>517</v>
-      </c>
       <c r="I104" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="105" spans="1:10" ht="195" x14ac:dyDescent="0.25">
@@ -5852,28 +5851,28 @@
         <v>104</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C105" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="D105">
         <v>2018</v>
       </c>
       <c r="E105" t="s">
+        <v>518</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="G105" t="s">
         <v>519</v>
       </c>
-      <c r="F105" s="1" t="s">
-        <v>629</v>
-      </c>
-      <c r="G105" t="s">
+      <c r="H105" t="s">
         <v>520</v>
       </c>
-      <c r="H105" t="s">
-        <v>521</v>
-      </c>
       <c r="I105" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="106" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -5881,28 +5880,28 @@
         <v>105</v>
       </c>
       <c r="B106" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="C106" t="s">
         <v>522</v>
-      </c>
-      <c r="C106" t="s">
-        <v>523</v>
       </c>
       <c r="D106">
         <v>2018</v>
       </c>
       <c r="E106" t="s">
+        <v>523</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="G106" t="s">
         <v>524</v>
       </c>
-      <c r="F106" s="1" t="s">
-        <v>630</v>
-      </c>
-      <c r="G106" t="s">
+      <c r="H106" t="s">
         <v>525</v>
       </c>
-      <c r="H106" t="s">
-        <v>526</v>
-      </c>
       <c r="I106" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="107" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -5910,28 +5909,28 @@
         <v>106</v>
       </c>
       <c r="B107" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="C107" t="s">
         <v>527</v>
-      </c>
-      <c r="C107" t="s">
-        <v>528</v>
       </c>
       <c r="D107">
         <v>2018</v>
       </c>
       <c r="E107" t="s">
+        <v>528</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="G107" t="s">
         <v>529</v>
       </c>
-      <c r="F107" s="1" t="s">
-        <v>631</v>
-      </c>
-      <c r="G107" t="s">
+      <c r="H107" t="s">
         <v>530</v>
       </c>
-      <c r="H107" t="s">
-        <v>531</v>
-      </c>
       <c r="I107" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="108" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -5939,28 +5938,28 @@
         <v>107</v>
       </c>
       <c r="B108" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="C108" t="s">
         <v>532</v>
-      </c>
-      <c r="C108" t="s">
-        <v>533</v>
       </c>
       <c r="D108">
         <v>2018</v>
       </c>
       <c r="E108" t="s">
+        <v>533</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="G108" t="s">
         <v>534</v>
       </c>
-      <c r="F108" s="1" t="s">
-        <v>632</v>
-      </c>
-      <c r="G108" t="s">
+      <c r="H108" t="s">
         <v>535</v>
       </c>
-      <c r="H108" t="s">
-        <v>536</v>
-      </c>
       <c r="I108" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="109" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -5968,28 +5967,28 @@
         <v>108</v>
       </c>
       <c r="B109" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="C109" t="s">
         <v>537</v>
-      </c>
-      <c r="C109" t="s">
-        <v>538</v>
       </c>
       <c r="D109">
         <v>2018</v>
       </c>
       <c r="E109" t="s">
+        <v>538</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="G109" t="s">
         <v>539</v>
       </c>
-      <c r="F109" s="1" t="s">
-        <v>633</v>
-      </c>
-      <c r="G109" t="s">
+      <c r="H109" t="s">
         <v>540</v>
       </c>
-      <c r="H109" t="s">
-        <v>541</v>
-      </c>
       <c r="I109" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="110" spans="1:10" ht="195" x14ac:dyDescent="0.25">
@@ -5997,28 +5996,28 @@
         <v>109</v>
       </c>
       <c r="B110" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="C110" t="s">
         <v>542</v>
-      </c>
-      <c r="C110" t="s">
-        <v>543</v>
       </c>
       <c r="D110">
         <v>2018</v>
       </c>
       <c r="E110" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="G110" t="s">
+        <v>543</v>
+      </c>
+      <c r="H110" t="s">
         <v>544</v>
       </c>
-      <c r="H110" t="s">
+      <c r="I110" t="s">
         <v>545</v>
-      </c>
-      <c r="I110" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="111" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -6026,28 +6025,28 @@
         <v>110</v>
       </c>
       <c r="B111" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="C111" t="s">
         <v>547</v>
-      </c>
-      <c r="C111" t="s">
-        <v>548</v>
       </c>
       <c r="D111">
         <v>2018</v>
       </c>
       <c r="E111" t="s">
+        <v>548</v>
+      </c>
+      <c r="F111" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="F111" s="1" t="s">
+      <c r="G111" t="s">
         <v>550</v>
       </c>
-      <c r="G111" t="s">
+      <c r="H111" t="s">
         <v>551</v>
       </c>
-      <c r="H111" t="s">
+      <c r="I111" t="s">
         <v>552</v>
-      </c>
-      <c r="I111" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="112" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -6055,28 +6054,28 @@
         <v>111</v>
       </c>
       <c r="B112" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="C112" t="s">
         <v>554</v>
-      </c>
-      <c r="C112" t="s">
-        <v>555</v>
       </c>
       <c r="D112">
         <v>2018</v>
       </c>
       <c r="E112" t="s">
+        <v>555</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="G112" t="s">
         <v>556</v>
       </c>
-      <c r="F112" s="1" t="s">
-        <v>635</v>
-      </c>
-      <c r="G112" t="s">
+      <c r="H112" t="s">
         <v>557</v>
       </c>
-      <c r="H112" t="s">
-        <v>558</v>
-      </c>
       <c r="I112" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="113" spans="1:9" ht="195" x14ac:dyDescent="0.25">
@@ -6084,28 +6083,28 @@
         <v>112</v>
       </c>
       <c r="B113" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="C113" t="s">
         <v>559</v>
-      </c>
-      <c r="C113" t="s">
-        <v>560</v>
       </c>
       <c r="D113">
         <v>2018</v>
       </c>
       <c r="E113" t="s">
+        <v>560</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="G113" t="s">
         <v>561</v>
       </c>
-      <c r="F113" s="1" t="s">
-        <v>636</v>
-      </c>
-      <c r="G113" t="s">
+      <c r="H113" t="s">
         <v>562</v>
       </c>
-      <c r="H113" t="s">
-        <v>563</v>
-      </c>
       <c r="I113" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="114" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -6113,28 +6112,28 @@
         <v>113</v>
       </c>
       <c r="B114" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="C114" t="s">
         <v>564</v>
-      </c>
-      <c r="C114" t="s">
-        <v>565</v>
       </c>
       <c r="D114">
         <v>2018</v>
       </c>
       <c r="E114" t="s">
+        <v>565</v>
+      </c>
+      <c r="F114" s="1" t="s">
         <v>566</v>
       </c>
-      <c r="F114" s="1" t="s">
+      <c r="G114" t="s">
         <v>567</v>
       </c>
-      <c r="G114" t="s">
+      <c r="H114" t="s">
         <v>568</v>
       </c>
-      <c r="H114" t="s">
-        <v>569</v>
-      </c>
       <c r="I114" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="115" spans="1:9" ht="135" x14ac:dyDescent="0.25">
@@ -6142,28 +6141,28 @@
         <v>114</v>
       </c>
       <c r="B115" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="C115" t="s">
         <v>570</v>
-      </c>
-      <c r="C115" t="s">
-        <v>571</v>
       </c>
       <c r="D115">
         <v>2018</v>
       </c>
       <c r="E115" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G115" t="s">
+        <v>571</v>
+      </c>
+      <c r="H115" t="s">
         <v>572</v>
       </c>
-      <c r="H115" t="s">
+      <c r="I115" t="s">
         <v>573</v>
-      </c>
-      <c r="I115" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="116" spans="1:9" ht="180" x14ac:dyDescent="0.25">
@@ -6171,28 +6170,28 @@
         <v>115</v>
       </c>
       <c r="B116" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="C116" t="s">
         <v>575</v>
-      </c>
-      <c r="C116" t="s">
-        <v>576</v>
       </c>
       <c r="D116">
         <v>2018</v>
       </c>
       <c r="E116" t="s">
+        <v>576</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="G116" t="s">
         <v>577</v>
       </c>
-      <c r="F116" s="1" t="s">
-        <v>637</v>
-      </c>
-      <c r="G116" t="s">
+      <c r="H116" t="s">
         <v>578</v>
       </c>
-      <c r="H116" t="s">
-        <v>579</v>
-      </c>
       <c r="I116" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="117" spans="1:9" ht="150" x14ac:dyDescent="0.25">
@@ -6200,28 +6199,28 @@
         <v>116</v>
       </c>
       <c r="B117" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="C117" t="s">
         <v>580</v>
-      </c>
-      <c r="C117" t="s">
-        <v>581</v>
       </c>
       <c r="D117">
         <v>2018</v>
       </c>
       <c r="E117" t="s">
+        <v>581</v>
+      </c>
+      <c r="F117" s="1" t="s">
         <v>582</v>
       </c>
-      <c r="F117" s="1" t="s">
+      <c r="G117" t="s">
         <v>583</v>
       </c>
-      <c r="G117" t="s">
+      <c r="H117" t="s">
         <v>584</v>
       </c>
-      <c r="H117" t="s">
+      <c r="I117" t="s">
         <v>585</v>
-      </c>
-      <c r="I117" t="s">
-        <v>586</v>
       </c>
     </row>
     <row r="118" spans="1:9" ht="180" x14ac:dyDescent="0.25">
@@ -6229,28 +6228,28 @@
         <v>117</v>
       </c>
       <c r="B118" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="C118" t="s">
         <v>587</v>
-      </c>
-      <c r="C118" t="s">
-        <v>588</v>
       </c>
       <c r="D118">
         <v>2018</v>
       </c>
       <c r="E118" t="s">
+        <v>588</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="G118" t="s">
         <v>589</v>
       </c>
-      <c r="F118" s="1" t="s">
-        <v>638</v>
-      </c>
-      <c r="G118" t="s">
+      <c r="H118" t="s">
         <v>590</v>
       </c>
-      <c r="H118" t="s">
-        <v>591</v>
-      </c>
       <c r="I118" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="119" spans="1:9" ht="225" x14ac:dyDescent="0.25">
@@ -6258,28 +6257,28 @@
         <v>118</v>
       </c>
       <c r="B119" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="C119" t="s">
         <v>592</v>
-      </c>
-      <c r="C119" t="s">
-        <v>593</v>
       </c>
       <c r="D119">
         <v>2018</v>
       </c>
       <c r="E119" t="s">
+        <v>593</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="G119" t="s">
         <v>594</v>
       </c>
-      <c r="F119" s="1" t="s">
-        <v>639</v>
-      </c>
-      <c r="G119" t="s">
+      <c r="H119" t="s">
         <v>595</v>
       </c>
-      <c r="H119" t="s">
-        <v>596</v>
-      </c>
       <c r="I119" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="120" spans="1:9" ht="150" x14ac:dyDescent="0.25">
@@ -6287,28 +6286,28 @@
         <v>119</v>
       </c>
       <c r="B120" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="C120" t="s">
         <v>597</v>
-      </c>
-      <c r="C120" t="s">
-        <v>598</v>
       </c>
       <c r="D120">
         <v>2018</v>
       </c>
       <c r="E120" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="G120" t="s">
+        <v>598</v>
+      </c>
+      <c r="H120" t="s">
         <v>599</v>
       </c>
-      <c r="H120" t="s">
-        <v>600</v>
-      </c>
       <c r="I120" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Explore feature functions complete
</commit_message>
<xml_diff>
--- a/DataTables/catalog_final.xlsx
+++ b/DataTables/catalog_final.xlsx
@@ -606,9 +606,6 @@
     <t xml:space="preserve">Pocket Sci-Fi is part of Pocket Reads, a superb collection of quality books that really capture children's imaginations! Pocket Reads have fantastic breadth and variety of genre, with Pocket Facts, Pocket Tales and Pocket Chillers making up the rest of the collection of independent readers </t>
   </si>
   <si>
-    <t>https://books.google.com.my/books/content?id=PgF3hxeyTKgC&amp;printsec=frontcover&amp;img=1&amp;zoom=1&amp;imgtk=AFLRE70kPlwu5OiUdB4uPQEmxNfATn5MN6h1GHCupW8p9o-OuRJEqksG2y-AT412YCsb5Av_tRkDFy9Y2zYWIuk8QCFpZPNyGs8ozQDUa35WQwEiGnv4npaQYsmEoB_6ggtQ6bpK-92d</t>
-  </si>
-  <si>
     <t>pocketscifithefinalfrontier</t>
   </si>
   <si>
@@ -873,9 +870,6 @@
     <t xml:space="preserve">In this story a little boy born with blue skin is laughed at by all the other children. But he has an important lesson to teach them. </t>
   </si>
   <si>
-    <t>https://books.google.com.my/books/content?id=6-EZeJ4LF8oC&amp;printsec=frontcover&amp;img=1&amp;zoom=5&amp;edge=curl&amp;imgtk=AFLRE73P9ILo_7hOAlbXjYG0Q2q8ubUrwUH589BRBc3aPH7F-HJV2ClBWvoF_00yuqcTwhf1pxo4Vhp5wS3u2qwI49_UFxboLnUw6fILd1RTJ5-2aG8zltPCcCkF61wbgcYJv2Pnsps1</t>
-  </si>
-  <si>
     <t>thelittleblueboy</t>
   </si>
   <si>
@@ -901,9 +895,6 @@
   </si>
   <si>
     <t xml:space="preserve">The Five Find-outers have got 15 thrilling mysteries to solve. Join Fatty, Larry, Daisy, Pip, Bets and Buster the dog in puzzling out these riddles. </t>
-  </si>
-  <si>
-    <t>https://books.google.com.my/books/content?id=Iyx_AAAACAAJ&amp;printsec=frontcover&amp;img=1&amp;zoom=1&amp;imgtk=AFLRE72vzEh-kF1_ZrRjrkoH_sPm7jihbAaS_flwJxohZX5oSHDDslesytx32Lii-8h6Y3UCGJ7QD5iVONy3ZuawNv5Di8acj58Cg7-8i3WxOoYkrcbMvbGn15mcYyqhL92vLh72ywlM</t>
   </si>
   <si>
     <t>themysteryofthehiddenhouse</t>
@@ -1959,13 +1950,22 @@
   </si>
   <si>
     <t>genre</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/41Sx94Qm0DL._BO1,204,203,200_.jpg</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/I/5153OvjEbHL._AC_UL436_SEARCH212385_.jpg</t>
+  </si>
+  <si>
+    <t>https://d1w7fb2mkkr3kw.cloudfront.net/assets/images/book/lrg/9780/6022/9780602243210.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2096,6 +2096,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2398,7 +2406,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -2441,14 +2449,16 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -2482,6 +2492,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -2804,8 +2815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="F93" sqref="F93:F101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2817,7 +2828,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -2841,7 +2852,7 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="J1" t="s">
         <v>7</v>
@@ -2896,7 +2907,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="G3" t="s">
         <v>19</v>
@@ -2925,7 +2936,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="G4" t="s">
         <v>24</v>
@@ -3157,7 +3168,7 @@
         <v>69</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="G12" t="s">
         <v>70</v>
@@ -3273,7 +3284,7 @@
         <v>39</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="G16" t="s">
         <v>88</v>
@@ -3360,7 +3371,7 @@
         <v>100</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="G19" t="s">
         <v>101</v>
@@ -3476,7 +3487,7 @@
         <v>124</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="G23" t="s">
         <v>125</v>
@@ -3592,7 +3603,7 @@
         <v>55</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="G27" t="s">
         <v>145</v>
@@ -3650,7 +3661,7 @@
         <v>55</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="G29" t="s">
         <v>153</v>
@@ -3708,7 +3719,7 @@
         <v>55</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="G31" t="s">
         <v>162</v>
@@ -3737,7 +3748,7 @@
         <v>55</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="G32" t="s">
         <v>166</v>
@@ -3853,7 +3864,7 @@
         <v>10</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="G36" t="s">
         <v>184</v>
@@ -3913,11 +3924,11 @@
       <c r="F38" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G38" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="H38" t="s">
         <v>195</v>
-      </c>
-      <c r="H38" t="s">
-        <v>196</v>
       </c>
       <c r="I38" t="s">
         <v>14</v>
@@ -3928,10 +3939,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C39" t="s">
         <v>197</v>
-      </c>
-      <c r="C39" t="s">
-        <v>198</v>
       </c>
       <c r="D39">
         <v>1995</v>
@@ -3940,13 +3951,13 @@
         <v>124</v>
       </c>
       <c r="F39" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="G39" t="s">
         <v>199</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>200</v>
-      </c>
-      <c r="H39" t="s">
-        <v>201</v>
       </c>
       <c r="I39" t="s">
         <v>21</v>
@@ -3957,10 +3968,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C40" t="s">
         <v>202</v>
-      </c>
-      <c r="C40" t="s">
-        <v>203</v>
       </c>
       <c r="D40" t="s">
         <v>10</v>
@@ -3969,13 +3980,13 @@
         <v>11</v>
       </c>
       <c r="F40" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G40" t="s">
         <v>204</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>205</v>
-      </c>
-      <c r="H40" t="s">
-        <v>206</v>
       </c>
       <c r="I40" t="s">
         <v>21</v>
@@ -3986,25 +3997,25 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C41" t="s">
         <v>207</v>
-      </c>
-      <c r="C41" t="s">
-        <v>208</v>
       </c>
       <c r="D41">
         <v>1995</v>
       </c>
       <c r="E41" t="s">
+        <v>208</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="G41" t="s">
         <v>210</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>211</v>
-      </c>
-      <c r="H41" t="s">
-        <v>212</v>
       </c>
       <c r="I41" t="s">
         <v>46</v>
@@ -4015,25 +4026,25 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C42" t="s">
         <v>213</v>
-      </c>
-      <c r="C42" t="s">
-        <v>214</v>
       </c>
       <c r="D42" t="s">
         <v>10</v>
       </c>
       <c r="E42" t="s">
+        <v>214</v>
+      </c>
+      <c r="F42" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="G42" t="s">
         <v>216</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>217</v>
-      </c>
-      <c r="H42" t="s">
-        <v>218</v>
       </c>
       <c r="I42" t="s">
         <v>59</v>
@@ -4044,10 +4055,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C43" t="s">
         <v>219</v>
-      </c>
-      <c r="C43" t="s">
-        <v>220</v>
       </c>
       <c r="D43">
         <v>2003</v>
@@ -4056,13 +4067,13 @@
         <v>39</v>
       </c>
       <c r="F43" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G43" t="s">
         <v>221</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H43" t="s">
         <v>222</v>
-      </c>
-      <c r="H43" t="s">
-        <v>223</v>
       </c>
       <c r="I43" t="s">
         <v>21</v>
@@ -4073,10 +4084,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C44" t="s">
         <v>224</v>
-      </c>
-      <c r="C44" t="s">
-        <v>225</v>
       </c>
       <c r="D44">
         <v>1993</v>
@@ -4085,16 +4096,16 @@
         <v>178</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="G44" t="s">
+        <v>225</v>
+      </c>
+      <c r="H44" t="s">
         <v>226</v>
       </c>
-      <c r="H44" t="s">
+      <c r="I44" t="s">
         <v>227</v>
-      </c>
-      <c r="I44" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -4102,25 +4113,25 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C45" t="s">
         <v>229</v>
-      </c>
-      <c r="C45" t="s">
-        <v>230</v>
       </c>
       <c r="D45">
         <v>2002</v>
       </c>
       <c r="E45" t="s">
+        <v>230</v>
+      </c>
+      <c r="F45" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="G45" t="s">
         <v>232</v>
       </c>
-      <c r="G45" t="s">
+      <c r="H45" t="s">
         <v>233</v>
-      </c>
-      <c r="H45" t="s">
-        <v>234</v>
       </c>
       <c r="I45" t="s">
         <v>14</v>
@@ -4131,25 +4142,25 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C46" t="s">
         <v>235</v>
-      </c>
-      <c r="C46" t="s">
-        <v>236</v>
       </c>
       <c r="D46">
         <v>2004</v>
       </c>
       <c r="E46" t="s">
+        <v>236</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="G46" t="s">
         <v>237</v>
       </c>
-      <c r="F46" s="1" t="s">
-        <v>612</v>
-      </c>
-      <c r="G46" t="s">
+      <c r="H46" t="s">
         <v>238</v>
-      </c>
-      <c r="H46" t="s">
-        <v>239</v>
       </c>
       <c r="I46" t="s">
         <v>116</v>
@@ -4160,25 +4171,25 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C47" t="s">
         <v>240</v>
-      </c>
-      <c r="C47" t="s">
-        <v>241</v>
       </c>
       <c r="D47">
         <v>2001</v>
       </c>
       <c r="E47" t="s">
+        <v>241</v>
+      </c>
+      <c r="F47" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="G47" t="s">
         <v>243</v>
       </c>
-      <c r="G47" t="s">
+      <c r="H47" t="s">
         <v>244</v>
-      </c>
-      <c r="H47" t="s">
-        <v>245</v>
       </c>
       <c r="I47" t="s">
         <v>109</v>
@@ -4189,25 +4200,25 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C48" t="s">
         <v>246</v>
-      </c>
-      <c r="C48" t="s">
-        <v>247</v>
       </c>
       <c r="D48">
         <v>1978</v>
       </c>
       <c r="E48" t="s">
+        <v>247</v>
+      </c>
+      <c r="F48" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="G48" t="s">
         <v>249</v>
       </c>
-      <c r="G48" t="s">
+      <c r="H48" t="s">
         <v>250</v>
-      </c>
-      <c r="H48" t="s">
-        <v>251</v>
       </c>
       <c r="I48" t="s">
         <v>59</v>
@@ -4218,25 +4229,25 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C49" t="s">
         <v>252</v>
-      </c>
-      <c r="C49" t="s">
-        <v>253</v>
       </c>
       <c r="D49">
         <v>2005</v>
       </c>
       <c r="E49" t="s">
+        <v>253</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="G49" t="s">
         <v>255</v>
       </c>
-      <c r="G49" t="s">
+      <c r="H49" t="s">
         <v>256</v>
-      </c>
-      <c r="H49" t="s">
-        <v>257</v>
       </c>
       <c r="I49" t="s">
         <v>36</v>
@@ -4247,25 +4258,25 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C50" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D50">
         <v>2003</v>
       </c>
       <c r="E50" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="G50" t="s">
+        <v>258</v>
+      </c>
+      <c r="H50" t="s">
         <v>259</v>
-      </c>
-      <c r="H50" t="s">
-        <v>260</v>
       </c>
       <c r="I50" t="s">
         <v>36</v>
@@ -4276,25 +4287,25 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C51" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D51">
         <v>2003</v>
       </c>
       <c r="E51" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="G51" t="s">
+        <v>261</v>
+      </c>
+      <c r="H51" t="s">
         <v>262</v>
-      </c>
-      <c r="H51" t="s">
-        <v>263</v>
       </c>
       <c r="I51" t="s">
         <v>36</v>
@@ -4305,25 +4316,25 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C52" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D52">
         <v>2003</v>
       </c>
       <c r="E52" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="G52" t="s">
+        <v>264</v>
+      </c>
+      <c r="H52" t="s">
         <v>265</v>
-      </c>
-      <c r="H52" t="s">
-        <v>266</v>
       </c>
       <c r="I52" t="s">
         <v>36</v>
@@ -4334,25 +4345,25 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C53" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D53">
         <v>2003</v>
       </c>
       <c r="E53" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F53" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="G53" t="s">
         <v>268</v>
       </c>
-      <c r="G53" t="s">
+      <c r="H53" t="s">
         <v>269</v>
-      </c>
-      <c r="H53" t="s">
-        <v>270</v>
       </c>
       <c r="I53" t="s">
         <v>36</v>
@@ -4363,25 +4374,25 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C54" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D54">
         <v>2003</v>
       </c>
       <c r="E54" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F54" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="G54" t="s">
         <v>272</v>
       </c>
-      <c r="G54" t="s">
+      <c r="H54" t="s">
         <v>273</v>
-      </c>
-      <c r="H54" t="s">
-        <v>274</v>
       </c>
       <c r="I54" t="s">
         <v>36</v>
@@ -4392,25 +4403,25 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C55" t="s">
         <v>275</v>
-      </c>
-      <c r="C55" t="s">
-        <v>276</v>
       </c>
       <c r="D55">
         <v>1966</v>
       </c>
       <c r="E55" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G55" t="s">
+        <v>277</v>
+      </c>
+      <c r="H55" t="s">
         <v>278</v>
-      </c>
-      <c r="H55" t="s">
-        <v>279</v>
       </c>
       <c r="I55" t="s">
         <v>72</v>
@@ -4421,25 +4432,25 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C56" t="s">
         <v>280</v>
-      </c>
-      <c r="C56" t="s">
-        <v>281</v>
       </c>
       <c r="D56">
         <v>1996</v>
       </c>
       <c r="E56" t="s">
+        <v>281</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="F56" s="1" t="s">
+      <c r="G56" s="2" t="s">
+        <v>644</v>
+      </c>
+      <c r="H56" t="s">
         <v>283</v>
-      </c>
-      <c r="G56" t="s">
-        <v>284</v>
-      </c>
-      <c r="H56" t="s">
-        <v>285</v>
       </c>
       <c r="I56" t="s">
         <v>14</v>
@@ -4450,10 +4461,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C57" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D57" t="s">
         <v>10</v>
@@ -4462,13 +4473,13 @@
         <v>11</v>
       </c>
       <c r="F57" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="G57" t="s">
+        <v>287</v>
+      </c>
+      <c r="H57" t="s">
         <v>288</v>
-      </c>
-      <c r="G57" t="s">
-        <v>289</v>
-      </c>
-      <c r="H57" t="s">
-        <v>290</v>
       </c>
       <c r="I57" t="s">
         <v>14</v>
@@ -4479,7 +4490,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C58" t="s">
         <v>31</v>
@@ -4488,16 +4499,16 @@
         <v>10</v>
       </c>
       <c r="E58" t="s">
+        <v>290</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>643</v>
+      </c>
+      <c r="H58" t="s">
         <v>292</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="G58" t="s">
-        <v>294</v>
-      </c>
-      <c r="H58" t="s">
-        <v>295</v>
       </c>
       <c r="I58" t="s">
         <v>36</v>
@@ -4508,25 +4519,25 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C59" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D59" t="s">
         <v>10</v>
       </c>
       <c r="E59" t="s">
+        <v>295</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="G59" t="s">
+        <v>297</v>
+      </c>
+      <c r="H59" t="s">
         <v>298</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="G59" t="s">
-        <v>300</v>
-      </c>
-      <c r="H59" t="s">
-        <v>301</v>
       </c>
       <c r="I59" t="s">
         <v>14</v>
@@ -4537,25 +4548,25 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C60" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D60">
         <v>2000</v>
       </c>
       <c r="E60" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="G60" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="H60" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="I60" t="s">
         <v>52</v>
@@ -4566,7 +4577,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C61" t="s">
         <v>161</v>
@@ -4578,13 +4589,13 @@
         <v>55</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="G61" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="H61" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="I61" t="s">
         <v>59</v>
@@ -4595,25 +4606,25 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C62" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D62">
         <v>2009</v>
       </c>
       <c r="E62" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="G62" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="H62" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I62" t="s">
         <v>109</v>
@@ -4624,7 +4635,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C63" t="s">
         <v>152</v>
@@ -4636,13 +4647,13 @@
         <v>55</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="G63" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="H63" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="I63" t="s">
         <v>59</v>
@@ -4653,25 +4664,25 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C64" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D64">
         <v>2004</v>
       </c>
       <c r="E64" t="s">
+        <v>319</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="G64" t="s">
+        <v>321</v>
+      </c>
+      <c r="H64" t="s">
         <v>322</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="G64" t="s">
-        <v>324</v>
-      </c>
-      <c r="H64" t="s">
-        <v>325</v>
       </c>
       <c r="I64" t="s">
         <v>21</v>
@@ -4682,10 +4693,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C65" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D65">
         <v>2002</v>
@@ -4694,13 +4705,13 @@
         <v>62</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="G65" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="H65" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="I65" t="s">
         <v>109</v>
@@ -4711,7 +4722,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C66" t="s">
         <v>10</v>
@@ -4723,13 +4734,13 @@
         <v>10</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="G66" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="H66" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="I66" t="s">
         <v>14</v>
@@ -4740,10 +4751,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C67" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D67">
         <v>1964</v>
@@ -4752,13 +4763,13 @@
         <v>11</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="G67" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="H67" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="I67" t="s">
         <v>21</v>
@@ -4769,10 +4780,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C68" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D68" t="s">
         <v>10</v>
@@ -4781,13 +4792,13 @@
         <v>11</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="G68" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="H68" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="I68" t="s">
         <v>21</v>
@@ -4798,10 +4809,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C69" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D69" t="s">
         <v>10</v>
@@ -4810,13 +4821,13 @@
         <v>11</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="G69" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="H69" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="I69" t="s">
         <v>21</v>
@@ -4827,28 +4838,28 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C70" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D70">
         <v>2002</v>
       </c>
       <c r="E70" t="s">
+        <v>349</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="G70" t="s">
+        <v>351</v>
+      </c>
+      <c r="H70" t="s">
         <v>352</v>
       </c>
-      <c r="F70" s="1" t="s">
+      <c r="I70" t="s">
         <v>353</v>
-      </c>
-      <c r="G70" t="s">
-        <v>354</v>
-      </c>
-      <c r="H70" t="s">
-        <v>355</v>
-      </c>
-      <c r="I70" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -4856,25 +4867,25 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C71" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="D71">
         <v>2011</v>
       </c>
       <c r="E71" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="G71" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="H71" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="I71" t="s">
         <v>109</v>
@@ -4885,7 +4896,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C72" t="s">
         <v>10</v>
@@ -4894,16 +4905,16 @@
         <v>1998</v>
       </c>
       <c r="E72" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="G72" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="H72" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="I72" t="s">
         <v>14</v>
@@ -4914,25 +4925,25 @@
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C73" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="D73">
         <v>2000</v>
       </c>
       <c r="E73" t="s">
+        <v>364</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="G73" t="s">
+        <v>366</v>
+      </c>
+      <c r="H73" t="s">
         <v>367</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="G73" t="s">
-        <v>369</v>
-      </c>
-      <c r="H73" t="s">
-        <v>370</v>
       </c>
       <c r="I73" t="s">
         <v>14</v>
@@ -4943,28 +4954,28 @@
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="C74" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D74">
         <v>2004</v>
       </c>
       <c r="E74" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F74" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="G74" t="s">
+        <v>371</v>
+      </c>
+      <c r="H74" t="s">
+        <v>372</v>
+      </c>
+      <c r="I74" t="s">
         <v>373</v>
-      </c>
-      <c r="G74" t="s">
-        <v>374</v>
-      </c>
-      <c r="H74" t="s">
-        <v>375</v>
-      </c>
-      <c r="I74" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -4972,28 +4983,28 @@
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C75" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D75">
         <v>2006</v>
       </c>
       <c r="E75" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="G75" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="H75" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="I75" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -5001,28 +5012,28 @@
         <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C76" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D76">
         <v>2011</v>
       </c>
       <c r="E76" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="G76" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H76" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="I76" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="105" x14ac:dyDescent="0.25">
@@ -5030,28 +5041,28 @@
         <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C77" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D77">
         <v>2010</v>
       </c>
       <c r="E77" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="G77" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="H77" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="I77" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -5059,28 +5070,28 @@
         <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="C78" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D78">
         <v>2010</v>
       </c>
       <c r="E78" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="G78" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="H78" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="I78" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -5088,28 +5099,28 @@
         <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C79" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D79">
         <v>2011</v>
       </c>
       <c r="E79" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="G79" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="H79" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="I79" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -5117,28 +5128,28 @@
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C80" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D80">
         <v>2011</v>
       </c>
       <c r="E80" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="G80" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="H80" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="I80" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -5146,28 +5157,28 @@
         <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C81" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D81">
         <v>2003</v>
       </c>
       <c r="E81" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="G81" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="H81" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="I81" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -5175,28 +5186,28 @@
         <v>81</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="C82" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D82">
         <v>2004</v>
       </c>
       <c r="E82" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="G82" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="H82" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="I82" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
@@ -5204,10 +5215,10 @@
         <v>82</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="C83" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D83" t="s">
         <v>10</v>
@@ -5216,13 +5227,13 @@
         <v>124</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="G83" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="H83" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="I83" t="s">
         <v>14</v>
@@ -5233,7 +5244,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C84" t="s">
         <v>31</v>
@@ -5242,16 +5253,16 @@
         <v>2001</v>
       </c>
       <c r="E84" t="s">
+        <v>412</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="G84" t="s">
+        <v>414</v>
+      </c>
+      <c r="H84" t="s">
         <v>415</v>
-      </c>
-      <c r="F84" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="G84" t="s">
-        <v>417</v>
-      </c>
-      <c r="H84" t="s">
-        <v>418</v>
       </c>
       <c r="I84" t="s">
         <v>14</v>
@@ -5262,7 +5273,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="C85" t="s">
         <v>31</v>
@@ -5271,16 +5282,16 @@
         <v>2001</v>
       </c>
       <c r="E85" t="s">
+        <v>417</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="G85" t="s">
+        <v>419</v>
+      </c>
+      <c r="H85" t="s">
         <v>420</v>
-      </c>
-      <c r="F85" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="G85" t="s">
-        <v>422</v>
-      </c>
-      <c r="H85" t="s">
-        <v>423</v>
       </c>
       <c r="I85" t="s">
         <v>14</v>
@@ -5291,7 +5302,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="C86" t="s">
         <v>31</v>
@@ -5300,16 +5311,16 @@
         <v>2001</v>
       </c>
       <c r="E86" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="G86" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H86" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="I86" t="s">
         <v>14</v>
@@ -5320,10 +5331,10 @@
         <v>86</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="C87" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="D87">
         <v>2005</v>
@@ -5332,13 +5343,13 @@
         <v>62</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="G87" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="H87" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I87" t="s">
         <v>14</v>
@@ -5349,25 +5360,25 @@
         <v>87</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C88" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="D88">
         <v>2009</v>
       </c>
       <c r="E88" t="s">
+        <v>432</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="G88" t="s">
+        <v>434</v>
+      </c>
+      <c r="H88" t="s">
         <v>435</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="G88" t="s">
-        <v>437</v>
-      </c>
-      <c r="H88" t="s">
-        <v>438</v>
       </c>
       <c r="I88" t="s">
         <v>46</v>
@@ -5378,25 +5389,25 @@
         <v>88</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="C89" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="D89">
         <v>1999</v>
       </c>
       <c r="E89" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="G89" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="H89" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="I89" t="s">
         <v>59</v>
@@ -5407,25 +5418,25 @@
         <v>89</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="C90" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="D90">
         <v>1973</v>
       </c>
       <c r="E90" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="G90" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="H90" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="I90" t="s">
         <v>142</v>
@@ -5436,25 +5447,25 @@
         <v>90</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="C91" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="D91">
         <v>2006</v>
       </c>
       <c r="E91" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="G91" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="H91" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="I91" t="s">
         <v>109</v>
@@ -5465,25 +5476,25 @@
         <v>91</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="C92" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="D92" t="s">
         <v>10</v>
       </c>
       <c r="E92" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="G92" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="H92" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="I92" t="s">
         <v>59</v>
@@ -5494,25 +5505,25 @@
         <v>92</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="C93" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="D93" t="s">
         <v>10</v>
       </c>
       <c r="E93" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G93" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="H93" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="I93" t="s">
         <v>59</v>
@@ -5523,25 +5534,25 @@
         <v>93</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="C94" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D94" t="s">
         <v>10</v>
       </c>
       <c r="E94" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="G94" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="H94" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="I94" t="s">
         <v>59</v>
@@ -5552,25 +5563,25 @@
         <v>94</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="C95" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D95">
         <v>2003</v>
       </c>
       <c r="E95" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="G95" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="H95" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="I95" t="s">
         <v>36</v>
@@ -5581,25 +5592,25 @@
         <v>95</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="C96" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D96">
         <v>2002</v>
       </c>
       <c r="E96" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="G96" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="H96" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="I96" t="s">
         <v>36</v>
@@ -5610,25 +5621,25 @@
         <v>96</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="C97" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D97">
         <v>2003</v>
       </c>
       <c r="E97" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="G97" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="H97" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="I97" t="s">
         <v>36</v>
@@ -5639,25 +5650,25 @@
         <v>97</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="C98" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D98">
         <v>2002</v>
       </c>
       <c r="E98" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="G98" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="H98" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="I98" t="s">
         <v>36</v>
@@ -5668,25 +5679,25 @@
         <v>98</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="C99" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="D99">
         <v>2002</v>
       </c>
       <c r="E99" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="G99" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="H99" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="I99" t="s">
         <v>72</v>
@@ -5697,25 +5708,25 @@
         <v>99</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="C100" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="D100">
         <v>2006</v>
       </c>
       <c r="E100" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="G100" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="H100" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="I100" t="s">
         <v>72</v>
@@ -5726,31 +5737,31 @@
         <v>100</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="C101" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="D101">
         <v>2018</v>
       </c>
       <c r="E101" t="s">
+        <v>492</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="G101" t="s">
+        <v>494</v>
+      </c>
+      <c r="H101" t="s">
         <v>495</v>
       </c>
-      <c r="F101" s="1" t="s">
-        <v>644</v>
-      </c>
-      <c r="G101" t="s">
+      <c r="I101" t="s">
+        <v>496</v>
+      </c>
+      <c r="J101" t="s">
         <v>497</v>
-      </c>
-      <c r="H101" t="s">
-        <v>498</v>
-      </c>
-      <c r="I101" t="s">
-        <v>499</v>
-      </c>
-      <c r="J101" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="102" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -5758,31 +5769,31 @@
         <v>101</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="C102" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="D102">
         <v>2018</v>
       </c>
       <c r="E102" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="G102" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="H102" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="I102" t="s">
         <v>66</v>
       </c>
       <c r="J102" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="103" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -5790,31 +5801,31 @@
         <v>102</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="C103" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="D103">
         <v>2018</v>
       </c>
       <c r="E103" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="G103" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="H103" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="I103" t="s">
         <v>52</v>
       </c>
       <c r="J103" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
     <row r="104" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -5822,28 +5833,28 @@
         <v>103</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="C104" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="D104">
         <v>2018</v>
       </c>
       <c r="E104" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="G104" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="H104" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="I104" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="105" spans="1:10" ht="195" x14ac:dyDescent="0.25">
@@ -5851,28 +5862,28 @@
         <v>104</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="C105" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="D105">
         <v>2018</v>
       </c>
       <c r="E105" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="G105" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="H105" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="I105" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="106" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -5880,25 +5891,25 @@
         <v>105</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="C106" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="D106">
         <v>2018</v>
       </c>
       <c r="E106" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="G106" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="H106" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="I106" t="s">
         <v>36</v>
@@ -5909,25 +5920,25 @@
         <v>106</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="C107" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="D107">
         <v>2018</v>
       </c>
       <c r="E107" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="G107" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="H107" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="I107" t="s">
         <v>72</v>
@@ -5938,25 +5949,25 @@
         <v>107</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="C108" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="D108">
         <v>2018</v>
       </c>
       <c r="E108" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="G108" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="H108" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="I108" t="s">
         <v>72</v>
@@ -5967,25 +5978,25 @@
         <v>108</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="C109" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="D109">
         <v>2018</v>
       </c>
       <c r="E109" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="G109" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="H109" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="I109" t="s">
         <v>72</v>
@@ -5996,28 +6007,28 @@
         <v>109</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="C110" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="D110">
         <v>2018</v>
       </c>
       <c r="E110" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="G110" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="H110" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="I110" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="111" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -6025,28 +6036,28 @@
         <v>110</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="C111" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="D111">
         <v>2018</v>
       </c>
       <c r="E111" t="s">
+        <v>545</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="G111" t="s">
+        <v>547</v>
+      </c>
+      <c r="H111" t="s">
         <v>548</v>
       </c>
-      <c r="F111" s="1" t="s">
+      <c r="I111" t="s">
         <v>549</v>
-      </c>
-      <c r="G111" t="s">
-        <v>550</v>
-      </c>
-      <c r="H111" t="s">
-        <v>551</v>
-      </c>
-      <c r="I111" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="112" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -6054,25 +6065,25 @@
         <v>111</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="C112" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="D112">
         <v>2018</v>
       </c>
       <c r="E112" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="G112" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="H112" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="I112" t="s">
         <v>52</v>
@@ -6083,28 +6094,28 @@
         <v>112</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="C113" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="D113">
         <v>2018</v>
       </c>
       <c r="E113" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="G113" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="H113" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="I113" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
     </row>
     <row r="114" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -6112,25 +6123,25 @@
         <v>113</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="C114" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="D114">
         <v>2018</v>
       </c>
       <c r="E114" t="s">
+        <v>562</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="G114" t="s">
+        <v>564</v>
+      </c>
+      <c r="H114" t="s">
         <v>565</v>
-      </c>
-      <c r="F114" s="1" t="s">
-        <v>566</v>
-      </c>
-      <c r="G114" t="s">
-        <v>567</v>
-      </c>
-      <c r="H114" t="s">
-        <v>568</v>
       </c>
       <c r="I114" t="s">
         <v>59</v>
@@ -6141,28 +6152,28 @@
         <v>114</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="C115" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="D115">
         <v>2018</v>
       </c>
       <c r="E115" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="G115" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="H115" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="I115" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="116" spans="1:9" ht="180" x14ac:dyDescent="0.25">
@@ -6170,25 +6181,25 @@
         <v>115</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="C116" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="D116">
         <v>2018</v>
       </c>
       <c r="E116" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="G116" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="H116" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="I116" t="s">
         <v>52</v>
@@ -6199,28 +6210,28 @@
         <v>116</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="C117" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="D117">
         <v>2018</v>
       </c>
       <c r="E117" t="s">
+        <v>578</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="G117" t="s">
+        <v>580</v>
+      </c>
+      <c r="H117" t="s">
         <v>581</v>
       </c>
-      <c r="F117" s="1" t="s">
+      <c r="I117" t="s">
         <v>582</v>
-      </c>
-      <c r="G117" t="s">
-        <v>583</v>
-      </c>
-      <c r="H117" t="s">
-        <v>584</v>
-      </c>
-      <c r="I117" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="118" spans="1:9" ht="180" x14ac:dyDescent="0.25">
@@ -6228,28 +6239,28 @@
         <v>117</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="C118" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="D118">
         <v>2018</v>
       </c>
       <c r="E118" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="G118" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="H118" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="I118" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="119" spans="1:9" ht="225" x14ac:dyDescent="0.25">
@@ -6257,28 +6268,28 @@
         <v>118</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="C119" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="D119">
         <v>2018</v>
       </c>
       <c r="E119" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="G119" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="H119" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="I119" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
     </row>
     <row r="120" spans="1:9" ht="150" x14ac:dyDescent="0.25">
@@ -6286,32 +6297,37 @@
         <v>119</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="C120" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="D120">
         <v>2018</v>
       </c>
       <c r="E120" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="G120" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="H120" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="I120" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G58" r:id="rId1"/>
+    <hyperlink ref="G56" r:id="rId2"/>
+    <hyperlink ref="G38" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>